<commit_message>
servicenow + updated models
</commit_message>
<xml_diff>
--- a/cybersecurity_stocks.xlsx
+++ b/cybersecurity_stocks.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jacharles\Desktop\work\models\financial_models\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32E88EB0-620D-4BB2-AA18-E85DCA69ED1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5E5FCF9-3B42-46EB-B776-CE6FB4E3D37F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19410" yWindow="1215" windowWidth="18555" windowHeight="19155" xr2:uid="{C49D2964-27D1-4A91-99C8-4FCFD2A434B5}"/>
+    <workbookView xWindow="14310" yWindow="0" windowWidth="19020" windowHeight="19155" xr2:uid="{C49D2964-27D1-4A91-99C8-4FCFD2A434B5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -933,7 +933,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D20" sqref="D20"/>
+      <selection pane="bottomLeft" activeCell="E45" sqref="E45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1591,7 +1591,7 @@
         <v>2239</v>
       </c>
       <c r="E45">
-        <v>110.17</v>
+        <v>14</v>
       </c>
       <c r="F45" t="s">
         <v>149</v>

</xml_diff>

<commit_message>
q3 '24 and earnings call notes for rapi7. added more cybersecu stocks
</commit_message>
<xml_diff>
--- a/cybersecurity_stocks.xlsx
+++ b/cybersecurity_stocks.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jacharles\Desktop\work\models\financial_models\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5E5FCF9-3B42-46EB-B776-CE6FB4E3D37F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2C21A54-AA49-4F00-A8D1-1D3714562652}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14310" yWindow="0" windowWidth="19020" windowHeight="19155" xr2:uid="{C49D2964-27D1-4A91-99C8-4FCFD2A434B5}"/>
+    <workbookView xWindow="19860" yWindow="30" windowWidth="18315" windowHeight="20850" xr2:uid="{C49D2964-27D1-4A91-99C8-4FCFD2A434B5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="178">
   <si>
     <t>Cyber Security Stock List</t>
   </si>
@@ -522,6 +522,54 @@
   </si>
   <si>
     <t xml:space="preserve">cloud  security. </t>
+  </si>
+  <si>
+    <t>Bottomline Technologies</t>
+  </si>
+  <si>
+    <t>EPAY</t>
+  </si>
+  <si>
+    <t>FLYW</t>
+  </si>
+  <si>
+    <t>AvePoinbt Inc</t>
+  </si>
+  <si>
+    <t>AVPT</t>
+  </si>
+  <si>
+    <t>Teradata Corp</t>
+  </si>
+  <si>
+    <t>TDC</t>
+  </si>
+  <si>
+    <t>Five9 Inc</t>
+  </si>
+  <si>
+    <t>FIVN</t>
+  </si>
+  <si>
+    <t>Progress Software Corp</t>
+  </si>
+  <si>
+    <t>PRGS</t>
+  </si>
+  <si>
+    <t>Calix Inc</t>
+  </si>
+  <si>
+    <t>CALX</t>
+  </si>
+  <si>
+    <t>Appian Corp</t>
+  </si>
+  <si>
+    <t>APPN</t>
+  </si>
+  <si>
+    <t>Flywire Corporation</t>
   </si>
 </sst>
 </file>
@@ -929,11 +977,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4FCF080F-901D-4273-8A5B-3493B71950B1}">
-  <dimension ref="A2:F57"/>
+  <dimension ref="A2:F66"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E45" sqref="E45"/>
+      <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1780,6 +1828,127 @@
         <v>161</v>
       </c>
     </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>162</v>
+      </c>
+      <c r="B58" t="s">
+        <v>163</v>
+      </c>
+      <c r="C58" s="5"/>
+      <c r="D58" s="6"/>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>177</v>
+      </c>
+      <c r="B59" t="s">
+        <v>164</v>
+      </c>
+      <c r="C59" s="5">
+        <v>23.17</v>
+      </c>
+      <c r="D59" s="6">
+        <v>2882</v>
+      </c>
+      <c r="E59">
+        <v>136.29</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>165</v>
+      </c>
+      <c r="B60" t="s">
+        <v>166</v>
+      </c>
+      <c r="C60" s="5">
+        <v>15.7</v>
+      </c>
+      <c r="D60" s="6">
+        <v>2944</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>167</v>
+      </c>
+      <c r="B61" t="s">
+        <v>168</v>
+      </c>
+      <c r="C61" s="5">
+        <v>29.79</v>
+      </c>
+      <c r="D61" s="6">
+        <v>2851</v>
+      </c>
+      <c r="E61">
+        <v>35.049999999999997</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>169</v>
+      </c>
+      <c r="B62" t="s">
+        <v>170</v>
+      </c>
+      <c r="C62" s="5">
+        <v>39.67</v>
+      </c>
+      <c r="D62" s="6">
+        <v>2984</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>171</v>
+      </c>
+      <c r="B63" t="s">
+        <v>172</v>
+      </c>
+      <c r="C63" s="5">
+        <v>68.28</v>
+      </c>
+      <c r="D63" s="6">
+        <v>2929</v>
+      </c>
+      <c r="E63">
+        <v>36.71</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>173</v>
+      </c>
+      <c r="B64" t="s">
+        <v>174</v>
+      </c>
+      <c r="C64" s="5">
+        <v>33.270000000000003</v>
+      </c>
+      <c r="D64" s="6">
+        <v>2206</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>175</v>
+      </c>
+      <c r="B65" t="s">
+        <v>176</v>
+      </c>
+      <c r="C65" s="5">
+        <v>40.28</v>
+      </c>
+      <c r="D65" s="6">
+        <v>2976</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C66" s="5"/>
+      <c r="D66" s="6"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
more stocks and updating the cybersecurity stock list
</commit_message>
<xml_diff>
--- a/cybersecurity_stocks.xlsx
+++ b/cybersecurity_stocks.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jacharles\Desktop\work\models\financial_models\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51855261-637A-4459-A762-EA6E5820F751}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{572C83CE-8F6F-4C6E-B726-2A50A133F5CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19095" yWindow="0" windowWidth="19410" windowHeight="20985" xr2:uid="{C49D2964-27D1-4A91-99C8-4FCFD2A434B5}"/>
+    <workbookView xWindow="14865" yWindow="675" windowWidth="16605" windowHeight="20850" xr2:uid="{C49D2964-27D1-4A91-99C8-4FCFD2A434B5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1001,8 +1001,8 @@
   <dimension ref="A2:K66"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D41" sqref="D41"/>
+      <pane ySplit="4" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A51" sqref="A51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1478,31 +1478,34 @@
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
+      <c r="A34" s="8" t="s">
         <v>33</v>
       </c>
       <c r="B34" t="s">
         <v>87</v>
       </c>
       <c r="C34" s="5">
-        <v>74.819999999999993</v>
+        <v>89.82</v>
       </c>
       <c r="D34" s="6">
-        <v>12709</v>
+        <v>14000</v>
       </c>
       <c r="F34" t="s">
         <v>138</v>
       </c>
+      <c r="G34" s="9">
+        <v>45715</v>
+      </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
+      <c r="A35" s="8" t="s">
         <v>34</v>
       </c>
       <c r="B35" t="s">
         <v>88</v>
       </c>
       <c r="C35" s="5">
-        <v>192</v>
+        <v>187.65</v>
       </c>
       <c r="D35" s="6">
         <v>122045</v>
@@ -1512,6 +1515,9 @@
       </c>
       <c r="F35" t="s">
         <v>139</v>
+      </c>
+      <c r="G35" s="9">
+        <v>45715</v>
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.25">
@@ -1992,6 +1998,8 @@
     <hyperlink ref="A45" r:id="rId6" xr:uid="{32A044DB-3E24-4FC0-A173-11F61BA0F6F4}"/>
     <hyperlink ref="A43" r:id="rId7" xr:uid="{5CE19AC8-AC7E-4A78-94F0-887F70A389DE}"/>
     <hyperlink ref="A5" r:id="rId8" xr:uid="{C6BDDC4D-F39A-4CF6-AF9E-184C5E93925D}"/>
+    <hyperlink ref="A34" r:id="rId9" xr:uid="{EA701455-58F4-458E-9944-656648537727}"/>
+    <hyperlink ref="A35" r:id="rId10" xr:uid="{7D272045-0AF5-4E8E-BCAC-F4870CC3E92E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>